<commit_message>
aim 2 metadata extraction
</commit_message>
<xml_diff>
--- a/data/raw/globalmix_duplicate_id_10272022.xlsx
+++ b/data/raw/globalmix_duplicate_id_10272022.xlsx
@@ -3204,8 +3204,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010030475AF969E55247A43045A5AE471F2A" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="be4495e03880ee1de3a22912b749265e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f04990b7-c779-4996-8758-cf2ccdb0b103" xmlns:ns3="b3b681de-c1b0-42ee-9ae3-1c9752c70d36" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c2f4482a333be99ab2445da9ec363ba" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010030475AF969E55247A43045A5AE471F2A" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bc6a0bdcebdc37da707fd810d30e6150">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f04990b7-c779-4996-8758-cf2ccdb0b103" xmlns:ns3="b3b681de-c1b0-42ee-9ae3-1c9752c70d36" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="943aa753a08003b20280a28c9001763d" ns2:_="" ns3:_="">
     <xsd:import namespace="f04990b7-c779-4996-8758-cf2ccdb0b103"/>
     <xsd:import namespace="b3b681de-c1b0-42ee-9ae3-1c9752c70d36"/>
     <xsd:element name="properties">
@@ -3230,6 +3230,7 @@
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -3310,6 +3311,11 @@
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b3b681de-c1b0-42ee-9ae3-1c9752c70d36" elementFormDefault="qualified">
@@ -3475,7 +3481,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C47C3EE3-623F-43D6-8B60-562194269B32}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26E99BCC-09C2-4930-BE6D-A0397DA82E2F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>